<commit_message>
Working copy of the agents, but with some minor bugs.
</commit_message>
<xml_diff>
--- a/possible states.xlsx
+++ b/possible states.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\steve\programming\Python Learning\mancala\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C6E9032-2993-4F47-A387-6820483C467F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAC0E7D9-4F39-46C1-A7AD-5AC4E722174E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13896" windowHeight="8496" xr2:uid="{216F9079-FFA2-4B8B-94FE-292E3219B3E9}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{216F9079-FFA2-4B8B-94FE-292E3219B3E9}"/>
   </bookViews>
   <sheets>
     <sheet name="Player0" sheetId="1" r:id="rId1"/>
@@ -507,7 +507,7 @@
     <sheetView tabSelected="1" topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="A2" sqref="A2"/>
-      <selection pane="bottomLeft" activeCell="C59" sqref="C59"/>
+      <selection pane="bottomLeft" activeCell="P103" sqref="P103"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="7" x14ac:dyDescent="0.3"/>
@@ -751,7 +751,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="6" spans="1:19" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:19" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A6" s="3">
         <v>1</v>
       </c>
@@ -809,7 +809,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="7" spans="1:19" outlineLevel="2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:19" hidden="1" outlineLevel="2" x14ac:dyDescent="0.3">
       <c r="A7" s="3">
         <v>1</v>
       </c>
@@ -867,7 +867,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="8" spans="1:19" outlineLevel="3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:19" hidden="1" outlineLevel="3" x14ac:dyDescent="0.3">
       <c r="A8" s="3">
         <v>1</v>
       </c>
@@ -5423,7 +5423,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="87" spans="1:19" outlineLevel="3" collapsed="1" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:19" hidden="1" outlineLevel="3" collapsed="1" x14ac:dyDescent="0.3">
       <c r="A87" s="3">
         <v>1</v>
       </c>
@@ -5481,7 +5481,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="88" spans="1:19" outlineLevel="3" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:19" hidden="1" outlineLevel="3" x14ac:dyDescent="0.3">
       <c r="A88" s="3">
         <v>1</v>
       </c>
@@ -5539,7 +5539,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="89" spans="1:19" outlineLevel="3" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:19" hidden="1" outlineLevel="3" x14ac:dyDescent="0.3">
       <c r="A89" s="3">
         <v>1</v>
       </c>
@@ -5597,7 +5597,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="90" spans="1:19" outlineLevel="3" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:19" hidden="1" outlineLevel="3" x14ac:dyDescent="0.3">
       <c r="A90" s="3">
         <v>1</v>
       </c>
@@ -5655,7 +5655,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="91" spans="1:19" outlineLevel="3" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:19" hidden="1" outlineLevel="3" x14ac:dyDescent="0.3">
       <c r="A91" s="3">
         <v>1</v>
       </c>
@@ -5713,7 +5713,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="92" spans="1:19" outlineLevel="2" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:19" hidden="1" outlineLevel="2" x14ac:dyDescent="0.3">
       <c r="A92" s="3">
         <v>1</v>
       </c>
@@ -5771,7 +5771,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="93" spans="1:19" outlineLevel="2" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:19" hidden="1" outlineLevel="2" x14ac:dyDescent="0.3">
       <c r="A93" s="3">
         <v>1</v>
       </c>
@@ -5828,7 +5828,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="94" spans="1:19" outlineLevel="2" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:19" hidden="1" outlineLevel="2" x14ac:dyDescent="0.3">
       <c r="A94" s="3">
         <v>1</v>
       </c>
@@ -5886,7 +5886,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="95" spans="1:19" outlineLevel="2" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:19" hidden="1" outlineLevel="2" x14ac:dyDescent="0.3">
       <c r="A95" s="3">
         <v>1</v>
       </c>
@@ -5944,7 +5944,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="96" spans="1:19" outlineLevel="2" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:19" hidden="1" outlineLevel="2" x14ac:dyDescent="0.3">
       <c r="A96" s="3">
         <v>1</v>
       </c>
@@ -6002,7 +6002,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="97" spans="1:19" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:19" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A97" s="3">
         <v>1</v>
       </c>
@@ -6060,7 +6060,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="98" spans="1:19" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:19" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A98" s="3">
         <v>1</v>
       </c>
@@ -6118,7 +6118,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="99" spans="1:19" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:19" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A99" s="3">
         <v>1</v>
       </c>
@@ -6176,7 +6176,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="100" spans="1:19" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:19" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A100" s="3">
         <v>1</v>
       </c>
@@ -6234,7 +6234,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="101" spans="1:19" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:19" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A101" s="3">
         <v>1</v>
       </c>
@@ -6292,7 +6292,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="102" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:19" collapsed="1" x14ac:dyDescent="0.3">
       <c r="A102" s="3">
         <v>1</v>
       </c>

</xml_diff>